<commit_message>
Ultima y nos vamos
</commit_message>
<xml_diff>
--- a/revisiones/Revisiones.xlsx
+++ b/revisiones/Revisiones.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lizbe\Documents\TheGroceries\revisiones\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{698624CE-6BC4-405E-800C-EC085CE352D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09314996-9A54-4162-AB1E-7A610137DE13}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" firstSheet="3" activeTab="3" xr2:uid="{D3B94AEF-2A3F-4005-A373-7D51D4B82D1D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" firstSheet="6" activeTab="8" xr2:uid="{D3B94AEF-2A3F-4005-A373-7D51D4B82D1D}"/>
   </bookViews>
   <sheets>
     <sheet name="Revisión 1 - COMPLETA" sheetId="1" r:id="rId1"/>
@@ -1585,8 +1585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D380BA2-8FD3-444F-9CB4-D1D45589F1D9}">
   <dimension ref="A1:K54"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2236,7 +2236,7 @@
         <v>61</v>
       </c>
       <c r="C50" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D50" s="11" t="s">
         <v>6</v>
@@ -2256,7 +2256,7 @@
         <v>63</v>
       </c>
       <c r="C51" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D51" s="11" t="s">
         <v>6</v>
@@ -2277,7 +2277,7 @@
         <v>64</v>
       </c>
       <c r="C52" s="24" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D52" s="12" t="s">
         <v>6</v>
@@ -2319,8 +2319,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{537904D1-DC81-4222-9809-557BF22DCA7B}">
   <dimension ref="A1:K117"/>
   <sheetViews>
-    <sheetView topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="E119" sqref="E119"/>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="C88" sqref="C88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2662,7 +2662,7 @@
         <v>71</v>
       </c>
       <c r="C28" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D28" s="11" t="s">
         <v>7</v>
@@ -2676,7 +2676,7 @@
         <v>71</v>
       </c>
       <c r="C29" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D29" s="11" t="s">
         <v>7</v>
@@ -2690,7 +2690,7 @@
         <v>23</v>
       </c>
       <c r="C30" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D30" s="11" t="s">
         <v>7</v>
@@ -2746,7 +2746,7 @@
         <v>28</v>
       </c>
       <c r="C34" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D34" s="11" t="s">
         <v>7</v>
@@ -2928,7 +2928,7 @@
         <v>68</v>
       </c>
       <c r="C47" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D47" s="11" t="s">
         <v>7</v>
@@ -3096,7 +3096,7 @@
         <v>71</v>
       </c>
       <c r="C59" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D59" s="11" t="s">
         <v>7</v>
@@ -3110,7 +3110,7 @@
         <v>71</v>
       </c>
       <c r="C60" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D60" s="11" t="s">
         <v>7</v>
@@ -3236,7 +3236,7 @@
         <v>68</v>
       </c>
       <c r="C69" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D69" s="11" t="s">
         <v>7</v>
@@ -3250,7 +3250,7 @@
         <v>73</v>
       </c>
       <c r="C70" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D70" s="11" t="s">
         <v>7</v>
@@ -3264,7 +3264,7 @@
         <v>71</v>
       </c>
       <c r="C71" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D71" s="11" t="s">
         <v>7</v>
@@ -3502,7 +3502,7 @@
         <v>71</v>
       </c>
       <c r="C88" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D88" s="11" t="s">
         <v>7</v>
@@ -3572,7 +3572,7 @@
         <v>79</v>
       </c>
       <c r="C93" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D93" s="11" t="s">
         <v>7</v>
@@ -3586,7 +3586,7 @@
         <v>68</v>
       </c>
       <c r="C94" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D94" s="11" t="s">
         <v>7</v>
@@ -3600,7 +3600,7 @@
         <v>69</v>
       </c>
       <c r="C95" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D95" s="11" t="s">
         <v>7</v>
@@ -3614,7 +3614,7 @@
         <v>71</v>
       </c>
       <c r="C96" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D96" s="11" t="s">
         <v>7</v>
@@ -3628,7 +3628,7 @@
         <v>71</v>
       </c>
       <c r="C97" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D97" s="11" t="s">
         <v>7</v>
@@ -3684,7 +3684,7 @@
         <v>80</v>
       </c>
       <c r="C101" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D101" s="11" t="s">
         <v>7</v>
@@ -3712,7 +3712,7 @@
         <v>81</v>
       </c>
       <c r="C103" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D103" s="11" t="s">
         <v>7</v>
@@ -3726,7 +3726,7 @@
         <v>82</v>
       </c>
       <c r="C104" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D104" s="11" t="s">
         <v>7</v>
@@ -3740,7 +3740,7 @@
         <v>83</v>
       </c>
       <c r="C105" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D105" s="11" t="s">
         <v>7</v>
@@ -3754,7 +3754,7 @@
         <v>84</v>
       </c>
       <c r="C106" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D106" s="11" t="s">
         <v>7</v>
@@ -3768,7 +3768,7 @@
         <v>85</v>
       </c>
       <c r="C107" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D107" s="11" t="s">
         <v>7</v>
@@ -3782,7 +3782,7 @@
         <v>86</v>
       </c>
       <c r="C108" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D108" s="11" t="s">
         <v>7</v>
@@ -3796,7 +3796,7 @@
         <v>87</v>
       </c>
       <c r="C109" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D109" s="11" t="s">
         <v>7</v>
@@ -3810,7 +3810,7 @@
         <v>88</v>
       </c>
       <c r="C110" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D110" s="11" t="s">
         <v>7</v>
@@ -3935,8 +3935,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76C58912-6208-4C9C-BB18-725D49522639}">
   <dimension ref="A1:K117"/>
   <sheetViews>
-    <sheetView topLeftCell="A108" workbookViewId="0">
-      <selection activeCell="D68" sqref="D68"/>
+    <sheetView topLeftCell="A121" workbookViewId="0">
+      <selection activeCell="C115" sqref="C115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4278,7 +4278,7 @@
         <v>71</v>
       </c>
       <c r="C28" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D28" s="11" t="s">
         <v>7</v>
@@ -4292,7 +4292,7 @@
         <v>71</v>
       </c>
       <c r="C29" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D29" s="11" t="s">
         <v>7</v>
@@ -4306,7 +4306,7 @@
         <v>23</v>
       </c>
       <c r="C30" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D30" s="11" t="s">
         <v>7</v>
@@ -4362,7 +4362,7 @@
         <v>28</v>
       </c>
       <c r="C34" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D34" s="11" t="s">
         <v>7</v>
@@ -4418,7 +4418,7 @@
         <v>68</v>
       </c>
       <c r="C38" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D38" s="11" t="s">
         <v>7</v>
@@ -4432,7 +4432,7 @@
         <v>69</v>
       </c>
       <c r="C39" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D39" s="11" t="s">
         <v>7</v>
@@ -4544,7 +4544,7 @@
         <v>68</v>
       </c>
       <c r="C47" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D47" s="11" t="s">
         <v>7</v>
@@ -4712,7 +4712,7 @@
         <v>71</v>
       </c>
       <c r="C59" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D59" s="11" t="s">
         <v>7</v>
@@ -4726,7 +4726,7 @@
         <v>71</v>
       </c>
       <c r="C60" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D60" s="11" t="s">
         <v>7</v>
@@ -4852,7 +4852,7 @@
         <v>68</v>
       </c>
       <c r="C69" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D69" s="11" t="s">
         <v>7</v>
@@ -4866,7 +4866,7 @@
         <v>73</v>
       </c>
       <c r="C70" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D70" s="11" t="s">
         <v>7</v>
@@ -4880,7 +4880,7 @@
         <v>71</v>
       </c>
       <c r="C71" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D71" s="11" t="s">
         <v>7</v>
@@ -5118,7 +5118,7 @@
         <v>71</v>
       </c>
       <c r="C88" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D88" s="11" t="s">
         <v>7</v>
@@ -5188,7 +5188,7 @@
         <v>79</v>
       </c>
       <c r="C93" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D93" s="11" t="s">
         <v>7</v>
@@ -5202,7 +5202,7 @@
         <v>68</v>
       </c>
       <c r="C94" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D94" s="11" t="s">
         <v>7</v>
@@ -5216,7 +5216,7 @@
         <v>69</v>
       </c>
       <c r="C95" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D95" s="11" t="s">
         <v>7</v>
@@ -5230,7 +5230,7 @@
         <v>71</v>
       </c>
       <c r="C96" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D96" s="11" t="s">
         <v>7</v>
@@ -5244,7 +5244,7 @@
         <v>71</v>
       </c>
       <c r="C97" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D97" s="11" t="s">
         <v>7</v>
@@ -5300,7 +5300,7 @@
         <v>80</v>
       </c>
       <c r="C101" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D101" s="11" t="s">
         <v>7</v>
@@ -5328,7 +5328,7 @@
         <v>81</v>
       </c>
       <c r="C103" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D103" s="11" t="s">
         <v>7</v>
@@ -5342,7 +5342,7 @@
         <v>82</v>
       </c>
       <c r="C104" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D104" s="11" t="s">
         <v>7</v>
@@ -5356,7 +5356,7 @@
         <v>83</v>
       </c>
       <c r="C105" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D105" s="11" t="s">
         <v>7</v>
@@ -5370,7 +5370,7 @@
         <v>84</v>
       </c>
       <c r="C106" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D106" s="11" t="s">
         <v>7</v>
@@ -5384,7 +5384,7 @@
         <v>85</v>
       </c>
       <c r="C107" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D107" s="11" t="s">
         <v>7</v>
@@ -5398,7 +5398,7 @@
         <v>86</v>
       </c>
       <c r="C108" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D108" s="11" t="s">
         <v>7</v>
@@ -5412,7 +5412,7 @@
         <v>87</v>
       </c>
       <c r="C109" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D109" s="11" t="s">
         <v>7</v>
@@ -5426,7 +5426,7 @@
         <v>88</v>
       </c>
       <c r="C110" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D110" s="11" t="s">
         <v>7</v>
@@ -5440,7 +5440,7 @@
         <v>89</v>
       </c>
       <c r="C111" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D111" s="11" t="s">
         <v>6</v>
@@ -5454,7 +5454,7 @@
         <v>50</v>
       </c>
       <c r="C112" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D112" s="11" t="s">
         <v>6</v>
@@ -5468,7 +5468,7 @@
         <v>55</v>
       </c>
       <c r="C113" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D113" s="11" t="s">
         <v>6</v>
@@ -5488,7 +5488,7 @@
         <v>91</v>
       </c>
       <c r="C114" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D114" s="11" t="s">
         <v>6</v>
@@ -5509,7 +5509,7 @@
         <v>92</v>
       </c>
       <c r="C115" s="24" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D115" s="12" t="s">
         <v>6</v>
@@ -5551,8 +5551,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD61CFE2-A61B-4156-BD0E-7D35F9B0B4F1}">
   <dimension ref="A1:K117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView topLeftCell="A113" workbookViewId="0">
+      <selection activeCell="C117" sqref="C117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5880,7 +5880,7 @@
         <v>69</v>
       </c>
       <c r="C27" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D27" s="11" t="s">
         <v>7</v>
@@ -5894,7 +5894,7 @@
         <v>102</v>
       </c>
       <c r="C28" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D28" s="11" t="s">
         <v>7</v>
@@ -5908,7 +5908,7 @@
         <v>25</v>
       </c>
       <c r="C29" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D29" s="11" t="s">
         <v>7</v>
@@ -5922,7 +5922,7 @@
         <v>26</v>
       </c>
       <c r="C30" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D30" s="11" t="s">
         <v>7</v>
@@ -5936,7 +5936,7 @@
         <v>27</v>
       </c>
       <c r="C31" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D31" s="11" t="s">
         <v>7</v>
@@ -5950,7 +5950,7 @@
         <v>71</v>
       </c>
       <c r="C32" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D32" s="11" t="s">
         <v>7</v>
@@ -5964,7 +5964,7 @@
         <v>103</v>
       </c>
       <c r="C33" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D33" s="11" t="s">
         <v>7</v>
@@ -5978,7 +5978,7 @@
         <v>23</v>
       </c>
       <c r="C34" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D34" s="11" t="s">
         <v>7</v>
@@ -5992,7 +5992,7 @@
         <v>15</v>
       </c>
       <c r="C35" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D35" s="11" t="s">
         <v>7</v>
@@ -6230,7 +6230,7 @@
         <v>71</v>
       </c>
       <c r="C52" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D52" s="11" t="s">
         <v>7</v>
@@ -6244,7 +6244,7 @@
         <v>107</v>
       </c>
       <c r="C53" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D53" s="11" t="s">
         <v>7</v>
@@ -6258,7 +6258,7 @@
         <v>71</v>
       </c>
       <c r="C54" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D54" s="11" t="s">
         <v>7</v>
@@ -6272,7 +6272,7 @@
         <v>113</v>
       </c>
       <c r="C55" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D55" s="11" t="s">
         <v>7</v>
@@ -6286,7 +6286,7 @@
         <v>73</v>
       </c>
       <c r="C56" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D56" s="11" t="s">
         <v>7</v>
@@ -6300,7 +6300,7 @@
         <v>116</v>
       </c>
       <c r="C57" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D57" s="11" t="s">
         <v>7</v>
@@ -6314,7 +6314,7 @@
         <v>117</v>
       </c>
       <c r="C58" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D58" s="11" t="s">
         <v>7</v>
@@ -6328,7 +6328,7 @@
         <v>68</v>
       </c>
       <c r="C59" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D59" s="11" t="s">
         <v>7</v>
@@ -6342,7 +6342,7 @@
         <v>71</v>
       </c>
       <c r="C60" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D60" s="11" t="s">
         <v>7</v>
@@ -6356,7 +6356,7 @@
         <v>25</v>
       </c>
       <c r="C61" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D61" s="11" t="s">
         <v>7</v>
@@ -6370,7 +6370,7 @@
         <v>15</v>
       </c>
       <c r="C62" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D62" s="11" t="s">
         <v>7</v>
@@ -6384,7 +6384,7 @@
         <v>118</v>
       </c>
       <c r="C63" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D63" s="11" t="s">
         <v>7</v>
@@ -6398,7 +6398,7 @@
         <v>103</v>
       </c>
       <c r="C64" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D64" s="11" t="s">
         <v>7</v>
@@ -6566,7 +6566,7 @@
         <v>71</v>
       </c>
       <c r="C76" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D76" s="11" t="s">
         <v>7</v>
@@ -6580,7 +6580,7 @@
         <v>59</v>
       </c>
       <c r="C77" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D77" s="11" t="s">
         <v>7</v>
@@ -6594,7 +6594,7 @@
         <v>79</v>
       </c>
       <c r="C78" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D78" s="11" t="s">
         <v>7</v>
@@ -6608,7 +6608,7 @@
         <v>26</v>
       </c>
       <c r="C79" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D79" s="11" t="s">
         <v>7</v>
@@ -6622,7 +6622,7 @@
         <v>68</v>
       </c>
       <c r="C80" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D80" s="11" t="s">
         <v>7</v>
@@ -6636,7 +6636,7 @@
         <v>69</v>
       </c>
       <c r="C81" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D81" s="11" t="s">
         <v>7</v>
@@ -6650,7 +6650,7 @@
         <v>71</v>
       </c>
       <c r="C82" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D82" s="11" t="s">
         <v>7</v>
@@ -6664,7 +6664,7 @@
         <v>118</v>
       </c>
       <c r="C83" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D83" s="11" t="s">
         <v>7</v>
@@ -6678,7 +6678,7 @@
         <v>111</v>
       </c>
       <c r="C84" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D84" s="11" t="s">
         <v>7</v>
@@ -6692,7 +6692,7 @@
         <v>71</v>
       </c>
       <c r="C85" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D85" s="11" t="s">
         <v>7</v>
@@ -6706,7 +6706,7 @@
         <v>25</v>
       </c>
       <c r="C86" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D86" s="11" t="s">
         <v>7</v>
@@ -6720,7 +6720,7 @@
         <v>103</v>
       </c>
       <c r="C87" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D87" s="11" t="s">
         <v>7</v>
@@ -6734,7 +6734,7 @@
         <v>26</v>
       </c>
       <c r="C88" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D88" s="11" t="s">
         <v>7</v>
@@ -6748,7 +6748,7 @@
         <v>120</v>
       </c>
       <c r="C89" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D89" s="11" t="s">
         <v>7</v>
@@ -6762,7 +6762,7 @@
         <v>121</v>
       </c>
       <c r="C90" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D90" s="11" t="s">
         <v>7</v>
@@ -6790,7 +6790,7 @@
         <v>81</v>
       </c>
       <c r="C92" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D92" s="11" t="s">
         <v>7</v>
@@ -6804,7 +6804,7 @@
         <v>82</v>
       </c>
       <c r="C93" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D93" s="11" t="s">
         <v>7</v>
@@ -6818,7 +6818,7 @@
         <v>83</v>
       </c>
       <c r="C94" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D94" s="11" t="s">
         <v>7</v>
@@ -6832,7 +6832,7 @@
         <v>85</v>
       </c>
       <c r="C95" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D95" s="11" t="s">
         <v>7</v>
@@ -6846,7 +6846,7 @@
         <v>86</v>
       </c>
       <c r="C96" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D96" s="11" t="s">
         <v>7</v>
@@ -6860,7 +6860,7 @@
         <v>110</v>
       </c>
       <c r="C97" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D97" s="11" t="s">
         <v>7</v>
@@ -6874,7 +6874,7 @@
         <v>87</v>
       </c>
       <c r="C98" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D98" s="11" t="s">
         <v>7</v>
@@ -6888,7 +6888,7 @@
         <v>88</v>
       </c>
       <c r="C99" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D99" s="11" t="s">
         <v>7</v>
@@ -6902,7 +6902,7 @@
         <v>122</v>
       </c>
       <c r="C100" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D100" s="11" t="s">
         <v>7</v>
@@ -6916,7 +6916,7 @@
         <v>123</v>
       </c>
       <c r="C101" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D101" s="11" t="s">
         <v>7</v>
@@ -6930,7 +6930,7 @@
         <v>124</v>
       </c>
       <c r="C102" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D102" s="11" t="s">
         <v>7</v>
@@ -6944,7 +6944,7 @@
         <v>92</v>
       </c>
       <c r="C103" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D103" s="11" t="s">
         <v>7</v>
@@ -6958,7 +6958,7 @@
         <v>125</v>
       </c>
       <c r="C104" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D104" s="11" t="s">
         <v>7</v>
@@ -6972,7 +6972,7 @@
         <v>115</v>
       </c>
       <c r="C105" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D105" s="11" t="s">
         <v>7</v>
@@ -6986,7 +6986,7 @@
         <v>71</v>
       </c>
       <c r="C106" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D106" s="11" t="s">
         <v>7</v>
@@ -7000,7 +7000,7 @@
         <v>125</v>
       </c>
       <c r="C107" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D107" s="11" t="s">
         <v>7</v>
@@ -7014,7 +7014,7 @@
         <v>127</v>
       </c>
       <c r="C108" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D108" s="11" t="s">
         <v>7</v>
@@ -7028,7 +7028,7 @@
         <v>81</v>
       </c>
       <c r="C109" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D109" s="11" t="s">
         <v>7</v>
@@ -7042,7 +7042,7 @@
         <v>129</v>
       </c>
       <c r="C110" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D110" s="11" t="s">
         <v>7</v>
@@ -7056,7 +7056,7 @@
         <v>110</v>
       </c>
       <c r="C111" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D111" s="11" t="s">
         <v>7</v>
@@ -7070,7 +7070,7 @@
         <v>122</v>
       </c>
       <c r="C112" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D112" s="11" t="s">
         <v>7</v>
@@ -7084,7 +7084,7 @@
         <v>92</v>
       </c>
       <c r="C113" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D113" s="11" t="s">
         <v>7</v>
@@ -7098,7 +7098,7 @@
         <v>125</v>
       </c>
       <c r="C114" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D114" s="11" t="s">
         <v>7</v>
@@ -7112,7 +7112,7 @@
         <v>115</v>
       </c>
       <c r="C115" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D115" s="11" t="s">
         <v>7</v>
@@ -7132,7 +7132,7 @@
         <v>71</v>
       </c>
       <c r="C116" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D116" s="11" t="s">
         <v>7</v>
@@ -7153,7 +7153,7 @@
         <v>125</v>
       </c>
       <c r="C117" s="24" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D117" s="12" t="s">
         <v>7</v>
@@ -7715,7 +7715,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E46F3F4-E61A-45DB-B136-E6C78C386E24}">
   <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
@@ -8304,7 +8304,7 @@
   <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8539,7 +8539,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B34E69A-292B-4DC2-9EEB-C9AFD6EFBE5D}">
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>

</xml_diff>